<commit_message>
Add Total Balance Component
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -83,6 +83,58 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3600450" y="876300"/>
+          <a:ext cx="3076575" cy="3876675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,7 +425,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -408,6 +460,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>